<commit_message>
Corte al miércoles 22/06/2022
</commit_message>
<xml_diff>
--- a/controlDiario.xlsx
+++ b/controlDiario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\AHK COORD INGLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E87371-FAAE-4316-BD1E-AF525FA304A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02E5714-B044-451C-BB53-16E763ADA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
   </bookViews>
   <sheets>
     <sheet name="ROSMAIRA (links)" sheetId="1" r:id="rId1"/>
@@ -943,7 +943,55 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Video estaba en proceso al momento de revisión el 21/06/2022 15H22.</t>
+Video estaba en proceso al momento de revisión el 21/06/2022 15H22 y al 22/09/2022 15H50.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M36" authorId="0" shapeId="0" xr:uid="{676B7302-6976-4A16-9EB9-5E42A13CEEA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Manuel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Video dura 00:03:13.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O36" authorId="0" shapeId="0" xr:uid="{233926BC-9CBE-4D57-B476-DAADC3613DD7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Manuel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Video estaba en proceso al momento de revisión el 22/06/2022 15H52.</t>
         </r>
       </text>
     </comment>
@@ -952,7 +1000,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="131">
   <si>
     <t>CURSO</t>
   </si>
@@ -1597,7 +1645,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1716,8 +1764,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1728,14 +1788,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1752,10 +1806,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2074,10 +2125,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2155,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -2114,7 +2166,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -2143,7 +2195,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -2154,7 +2206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -2165,7 +2217,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2228,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -2187,7 +2239,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -2198,7 +2250,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -2209,7 +2261,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -2220,7 +2272,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -2242,7 +2294,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -2254,7 +2306,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C16" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}"/>
+  <autoFilter ref="A2:C16" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="02_Martes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{A1EA6162-9F94-41F9-B581-C06B3AEA2E9D}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{773B485D-E09A-4C89-9A13-77122C44E990}"/>
@@ -2280,8 +2338,8 @@
   <dimension ref="A1:P115"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+      <pane ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,44 +2352,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2340,11 +2398,11 @@
       <c r="N3" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="55">
+      <c r="O3" s="57">
         <f ca="1">NOW()</f>
-        <v>44733.646704976854</v>
-      </c>
-      <c r="P3" s="56"/>
+        <v>44734.662150925928</v>
+      </c>
+      <c r="P3" s="58"/>
     </row>
     <row r="5" spans="1:16" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2400,7 +2458,7 @@
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="53">
         <v>1</v>
       </c>
       <c r="C6" s="12">
@@ -2448,7 +2506,7 @@
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="12">
         <v>1</v>
       </c>
@@ -2494,7 +2552,7 @@
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="12">
         <v>1</v>
       </c>
@@ -2540,7 +2598,7 @@
       <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="12">
         <v>1</v>
       </c>
@@ -2586,7 +2644,7 @@
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="51"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="12">
         <v>1</v>
       </c>
@@ -2632,7 +2690,7 @@
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="50">
         <v>2</v>
       </c>
       <c r="C11" s="6">
@@ -2680,7 +2738,7 @@
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="53"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="6">
         <v>6</v>
       </c>
@@ -2726,7 +2784,7 @@
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="53"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="5">
         <v>1</v>
       </c>
@@ -2772,7 +2830,7 @@
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="53"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="6"/>
       <c r="D14" s="22"/>
       <c r="E14" s="5"/>
@@ -2792,7 +2850,7 @@
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="53"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="6"/>
       <c r="D15" s="22"/>
       <c r="E15" s="5"/>
@@ -2812,7 +2870,7 @@
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="6">
         <v>1</v>
       </c>
@@ -2858,7 +2916,7 @@
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="6"/>
       <c r="D17" s="22"/>
       <c r="E17" s="5"/>
@@ -2878,7 +2936,7 @@
       <c r="A18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="53">
         <v>3</v>
       </c>
       <c r="C18" s="12">
@@ -2926,7 +2984,7 @@
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="12">
         <v>5</v>
       </c>
@@ -2972,7 +3030,7 @@
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="12">
         <v>1</v>
       </c>
@@ -3018,7 +3076,7 @@
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="12">
         <v>1</v>
       </c>
@@ -3064,7 +3122,7 @@
       <c r="A22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="12"/>
       <c r="D22" s="22"/>
       <c r="E22" s="12"/>
@@ -3084,7 +3142,7 @@
       <c r="A23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="50"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="12">
         <v>1</v>
       </c>
@@ -3130,7 +3188,7 @@
       <c r="A24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="51"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="12"/>
       <c r="D24" s="22"/>
       <c r="E24" s="13"/>
@@ -3150,7 +3208,7 @@
       <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="52">
+      <c r="B25" s="50">
         <v>4</v>
       </c>
       <c r="C25" s="34">
@@ -3198,7 +3256,7 @@
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="53"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="6">
         <v>2</v>
       </c>
@@ -3244,7 +3302,7 @@
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="53"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="6">
         <v>1</v>
       </c>
@@ -3290,7 +3348,7 @@
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="53"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="6"/>
       <c r="D28" s="22"/>
       <c r="E28" s="6"/>
@@ -3310,7 +3368,7 @@
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="53"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="6">
         <v>1</v>
       </c>
@@ -3356,7 +3414,7 @@
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="53"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="6"/>
       <c r="D30" s="22"/>
       <c r="E30" s="6"/>
@@ -3376,7 +3434,7 @@
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="54"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="6">
         <v>1</v>
       </c>
@@ -3422,15 +3480,19 @@
       <c r="A32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="49">
+      <c r="B32" s="53">
         <v>5</v>
       </c>
       <c r="C32" s="33">
         <v>1</v>
       </c>
       <c r="D32" s="21"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="E32" s="33">
+        <v>1</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1</v>
+      </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -3439,7 +3501,9 @@
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
+      <c r="O32" s="33">
+        <v>1</v>
+      </c>
       <c r="P32" s="33">
         <v>1</v>
       </c>
@@ -3448,13 +3512,17 @@
       <c r="A33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="50"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="12">
         <v>5</v>
       </c>
       <c r="D33" s="22"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="E33" s="12">
+        <v>5</v>
+      </c>
+      <c r="F33" s="12">
+        <v>5</v>
+      </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -3463,7 +3531,9 @@
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
+      <c r="O33" s="12">
+        <v>5</v>
+      </c>
       <c r="P33" s="12">
         <v>5</v>
       </c>
@@ -3472,13 +3542,17 @@
       <c r="A34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="50"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="12">
         <v>1</v>
       </c>
       <c r="D34" s="22"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="12">
+        <v>1</v>
+      </c>
+      <c r="F34" s="12">
+        <v>1</v>
+      </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
@@ -3487,7 +3561,9 @@
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
+      <c r="O34" s="12">
+        <v>1</v>
+      </c>
       <c r="P34" s="12">
         <v>1</v>
       </c>
@@ -3496,11 +3572,11 @@
       <c r="A35" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="50"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="12"/>
       <c r="D35" s="22"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -3509,18 +3585,18 @@
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
+      <c r="O35" s="12"/>
       <c r="P35" s="12"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="50"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="12"/>
       <c r="D36" s="22"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -3529,20 +3605,24 @@
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
+      <c r="O36" s="12"/>
       <c r="P36" s="12"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="50"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="12">
         <v>1</v>
       </c>
       <c r="D37" s="22"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
+        <v>1</v>
+      </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
@@ -3551,7 +3631,9 @@
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
+      <c r="O37" s="12">
+        <v>1</v>
+      </c>
       <c r="P37" s="12">
         <v>1</v>
       </c>
@@ -3560,7 +3642,7 @@
       <c r="A38" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="51"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="12"/>
       <c r="D38" s="22"/>
       <c r="E38" s="13"/>
@@ -3580,7 +3662,7 @@
       <c r="A39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="52">
+      <c r="B39" s="50">
         <v>6</v>
       </c>
       <c r="C39" s="9"/>
@@ -3602,7 +3684,7 @@
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="53"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="9"/>
       <c r="D40" s="22"/>
       <c r="E40" s="9"/>
@@ -3622,7 +3704,7 @@
       <c r="A41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="53"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="9"/>
       <c r="D41" s="22"/>
       <c r="E41" s="9"/>
@@ -3642,7 +3724,7 @@
       <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="53"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="9"/>
       <c r="D42" s="22"/>
       <c r="E42" s="5"/>
@@ -3662,7 +3744,7 @@
       <c r="A43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="53"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="9"/>
       <c r="D43" s="22"/>
       <c r="E43" s="5"/>
@@ -3682,7 +3764,7 @@
       <c r="A44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="53"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="9"/>
       <c r="D44" s="22"/>
       <c r="E44" s="5"/>
@@ -3702,7 +3784,7 @@
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="54"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="9"/>
       <c r="D45" s="22"/>
       <c r="E45" s="5"/>
@@ -3722,7 +3804,7 @@
       <c r="A46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="49">
+      <c r="B46" s="53">
         <v>7</v>
       </c>
       <c r="C46" s="11"/>
@@ -3744,7 +3826,7 @@
       <c r="A47" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="50"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="13"/>
       <c r="D47" s="22"/>
       <c r="E47" s="13"/>
@@ -3764,7 +3846,7 @@
       <c r="A48" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="50"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="13"/>
       <c r="D48" s="22"/>
       <c r="E48" s="13"/>
@@ -3784,7 +3866,7 @@
       <c r="A49" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="50"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="13"/>
       <c r="D49" s="22"/>
       <c r="E49" s="13"/>
@@ -3804,7 +3886,7 @@
       <c r="A50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="50"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="13"/>
       <c r="D50" s="22"/>
       <c r="E50" s="13"/>
@@ -3824,7 +3906,7 @@
       <c r="A51" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="50"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="13"/>
       <c r="D51" s="22"/>
       <c r="E51" s="13"/>
@@ -3844,7 +3926,7 @@
       <c r="A52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="51"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="13"/>
       <c r="D52" s="22"/>
       <c r="E52" s="13"/>
@@ -3864,7 +3946,7 @@
       <c r="A53" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="52">
+      <c r="B53" s="50">
         <v>8</v>
       </c>
       <c r="C53" s="5"/>
@@ -3886,7 +3968,7 @@
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="53"/>
+      <c r="B54" s="51"/>
       <c r="C54" s="5"/>
       <c r="D54" s="22"/>
       <c r="E54" s="5"/>
@@ -3906,7 +3988,7 @@
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="53"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="6"/>
       <c r="D55" s="21"/>
       <c r="E55" s="6"/>
@@ -3926,7 +4008,7 @@
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="53"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="6"/>
       <c r="D56" s="21"/>
       <c r="E56" s="5"/>
@@ -3946,7 +4028,7 @@
       <c r="A57" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="53"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="6"/>
       <c r="D57" s="21"/>
       <c r="E57" s="5"/>
@@ -3966,7 +4048,7 @@
       <c r="A58" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="53"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="6"/>
       <c r="D58" s="21"/>
       <c r="E58" s="5"/>
@@ -3986,7 +4068,7 @@
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="54"/>
+      <c r="B59" s="52"/>
       <c r="C59" s="6"/>
       <c r="D59" s="21"/>
       <c r="E59" s="6"/>
@@ -4006,7 +4088,7 @@
       <c r="A60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="49">
+      <c r="B60" s="53">
         <v>9</v>
       </c>
       <c r="C60" s="13"/>
@@ -4028,7 +4110,7 @@
       <c r="A61" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="50"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="13"/>
       <c r="D61" s="22"/>
       <c r="E61" s="13"/>
@@ -4048,7 +4130,7 @@
       <c r="A62" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="50"/>
+      <c r="B62" s="54"/>
       <c r="C62" s="13"/>
       <c r="D62" s="22"/>
       <c r="E62" s="13"/>
@@ -4068,7 +4150,7 @@
       <c r="A63" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="50"/>
+      <c r="B63" s="54"/>
       <c r="C63" s="13"/>
       <c r="D63" s="23"/>
       <c r="E63" s="10"/>
@@ -4088,7 +4170,7 @@
       <c r="A64" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B64" s="50"/>
+      <c r="B64" s="54"/>
       <c r="C64" s="13"/>
       <c r="D64" s="23"/>
       <c r="E64" s="10"/>
@@ -4108,7 +4190,7 @@
       <c r="A65" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="50"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="13"/>
       <c r="D65" s="23"/>
       <c r="E65" s="10"/>
@@ -4128,7 +4210,7 @@
       <c r="A66" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="51"/>
+      <c r="B66" s="55"/>
       <c r="C66" s="13"/>
       <c r="D66" s="23"/>
       <c r="E66" s="10"/>
@@ -4148,7 +4230,7 @@
       <c r="A67" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="52">
+      <c r="B67" s="50">
         <v>10</v>
       </c>
       <c r="C67" s="5"/>
@@ -4170,7 +4252,7 @@
       <c r="A68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="53"/>
+      <c r="B68" s="51"/>
       <c r="C68" s="5"/>
       <c r="D68" s="22"/>
       <c r="E68" s="5"/>
@@ -4190,7 +4272,7 @@
       <c r="A69" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="53"/>
+      <c r="B69" s="51"/>
       <c r="C69" s="5"/>
       <c r="D69" s="22"/>
       <c r="E69" s="5"/>
@@ -4210,7 +4292,7 @@
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="53"/>
+      <c r="B70" s="51"/>
       <c r="C70" s="5"/>
       <c r="D70" s="22"/>
       <c r="E70" s="5"/>
@@ -4230,7 +4312,7 @@
       <c r="A71" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="53"/>
+      <c r="B71" s="51"/>
       <c r="C71" s="5"/>
       <c r="D71" s="22"/>
       <c r="E71" s="5"/>
@@ -4250,7 +4332,7 @@
       <c r="A72" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="53"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="5"/>
       <c r="D72" s="22"/>
       <c r="E72" s="5"/>
@@ -4270,7 +4352,7 @@
       <c r="A73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="54"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="6"/>
       <c r="D73" s="21"/>
       <c r="E73" s="6"/>
@@ -4290,7 +4372,7 @@
       <c r="A74" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="49">
+      <c r="B74" s="53">
         <v>11</v>
       </c>
       <c r="C74" s="13"/>
@@ -4312,7 +4394,7 @@
       <c r="A75" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="50"/>
+      <c r="B75" s="54"/>
       <c r="C75" s="13"/>
       <c r="D75" s="22"/>
       <c r="E75" s="13"/>
@@ -4332,7 +4414,7 @@
       <c r="A76" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="50"/>
+      <c r="B76" s="54"/>
       <c r="C76" s="13"/>
       <c r="D76" s="22"/>
       <c r="E76" s="13"/>
@@ -4352,7 +4434,7 @@
       <c r="A77" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="50"/>
+      <c r="B77" s="54"/>
       <c r="C77" s="13"/>
       <c r="D77" s="22"/>
       <c r="E77" s="13"/>
@@ -4372,7 +4454,7 @@
       <c r="A78" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="50"/>
+      <c r="B78" s="54"/>
       <c r="C78" s="10"/>
       <c r="D78" s="23"/>
       <c r="E78" s="10"/>
@@ -4392,7 +4474,7 @@
       <c r="A79" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="50"/>
+      <c r="B79" s="54"/>
       <c r="C79" s="13"/>
       <c r="D79" s="22"/>
       <c r="E79" s="13"/>
@@ -4412,7 +4494,7 @@
       <c r="A80" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B80" s="51"/>
+      <c r="B80" s="55"/>
       <c r="C80" s="13"/>
       <c r="D80" s="23"/>
       <c r="E80" s="10"/>
@@ -4432,7 +4514,7 @@
       <c r="A81" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="52">
+      <c r="B81" s="50">
         <v>12</v>
       </c>
       <c r="C81" s="5"/>
@@ -4454,7 +4536,7 @@
       <c r="A82" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="53"/>
+      <c r="B82" s="51"/>
       <c r="C82" s="5"/>
       <c r="D82" s="22"/>
       <c r="E82" s="5"/>
@@ -4474,7 +4556,7 @@
       <c r="A83" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="53"/>
+      <c r="B83" s="51"/>
       <c r="C83" s="5"/>
       <c r="D83" s="22"/>
       <c r="E83" s="5"/>
@@ -4494,7 +4576,7 @@
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="53"/>
+      <c r="B84" s="51"/>
       <c r="C84" s="5"/>
       <c r="D84" s="22"/>
       <c r="E84" s="5"/>
@@ -4514,7 +4596,7 @@
       <c r="A85" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="53"/>
+      <c r="B85" s="51"/>
       <c r="C85" s="5"/>
       <c r="D85" s="22"/>
       <c r="E85" s="5"/>
@@ -4534,7 +4616,7 @@
       <c r="A86" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B86" s="53"/>
+      <c r="B86" s="51"/>
       <c r="C86" s="5"/>
       <c r="D86" s="22"/>
       <c r="E86" s="5"/>
@@ -4554,7 +4636,7 @@
       <c r="A87" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="54"/>
+      <c r="B87" s="52"/>
       <c r="C87" s="5"/>
       <c r="D87" s="22"/>
       <c r="E87" s="5"/>
@@ -4574,7 +4656,7 @@
       <c r="A88" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B88" s="49">
+      <c r="B88" s="53">
         <v>13</v>
       </c>
       <c r="C88" s="13"/>
@@ -4596,7 +4678,7 @@
       <c r="A89" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="50"/>
+      <c r="B89" s="54"/>
       <c r="C89" s="13"/>
       <c r="D89" s="22"/>
       <c r="E89" s="13"/>
@@ -4616,7 +4698,7 @@
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="50"/>
+      <c r="B90" s="54"/>
       <c r="C90" s="13"/>
       <c r="D90" s="22"/>
       <c r="E90" s="13"/>
@@ -4636,7 +4718,7 @@
       <c r="A91" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="50"/>
+      <c r="B91" s="54"/>
       <c r="C91" s="13"/>
       <c r="D91" s="22"/>
       <c r="E91" s="13"/>
@@ -4656,7 +4738,7 @@
       <c r="A92" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B92" s="50"/>
+      <c r="B92" s="54"/>
       <c r="C92" s="13"/>
       <c r="D92" s="22"/>
       <c r="E92" s="13"/>
@@ -4676,7 +4758,7 @@
       <c r="A93" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="50"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="13"/>
       <c r="D93" s="22"/>
       <c r="E93" s="13"/>
@@ -4696,7 +4778,7 @@
       <c r="A94" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B94" s="51"/>
+      <c r="B94" s="55"/>
       <c r="C94" s="13"/>
       <c r="D94" s="23"/>
       <c r="E94" s="10"/>
@@ -4716,7 +4798,7 @@
       <c r="A95" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="52">
+      <c r="B95" s="50">
         <v>14</v>
       </c>
       <c r="C95" s="16"/>
@@ -4738,7 +4820,7 @@
       <c r="A96" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B96" s="53"/>
+      <c r="B96" s="51"/>
       <c r="C96" s="16"/>
       <c r="D96" s="22"/>
       <c r="E96" s="16"/>
@@ -4758,7 +4840,7 @@
       <c r="A97" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="53"/>
+      <c r="B97" s="51"/>
       <c r="C97" s="16"/>
       <c r="D97" s="22"/>
       <c r="E97" s="16"/>
@@ -4778,7 +4860,7 @@
       <c r="A98" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="53"/>
+      <c r="B98" s="51"/>
       <c r="C98" s="16"/>
       <c r="D98" s="22"/>
       <c r="E98" s="16"/>
@@ -4798,7 +4880,7 @@
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B99" s="53"/>
+      <c r="B99" s="51"/>
       <c r="C99" s="16"/>
       <c r="D99" s="22"/>
       <c r="E99" s="16"/>
@@ -4818,7 +4900,7 @@
       <c r="A100" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B100" s="53"/>
+      <c r="B100" s="51"/>
       <c r="C100" s="16"/>
       <c r="D100" s="22"/>
       <c r="E100" s="16"/>
@@ -4838,7 +4920,7 @@
       <c r="A101" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="54"/>
+      <c r="B101" s="52"/>
       <c r="C101" s="16"/>
       <c r="D101" s="22"/>
       <c r="E101" s="16"/>
@@ -4858,7 +4940,7 @@
       <c r="A102" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="49">
+      <c r="B102" s="53">
         <v>15</v>
       </c>
       <c r="C102" s="13"/>
@@ -4880,7 +4962,7 @@
       <c r="A103" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B103" s="50"/>
+      <c r="B103" s="54"/>
       <c r="C103" s="13"/>
       <c r="D103" s="22"/>
       <c r="E103" s="13"/>
@@ -4900,7 +4982,7 @@
       <c r="A104" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="50"/>
+      <c r="B104" s="54"/>
       <c r="C104" s="13"/>
       <c r="D104" s="22"/>
       <c r="E104" s="13"/>
@@ -4920,7 +5002,7 @@
       <c r="A105" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="50"/>
+      <c r="B105" s="54"/>
       <c r="C105" s="13"/>
       <c r="D105" s="22"/>
       <c r="E105" s="13"/>
@@ -4940,7 +5022,7 @@
       <c r="A106" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B106" s="50"/>
+      <c r="B106" s="54"/>
       <c r="C106" s="13"/>
       <c r="D106" s="22"/>
       <c r="E106" s="13"/>
@@ -4960,7 +5042,7 @@
       <c r="A107" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B107" s="50"/>
+      <c r="B107" s="54"/>
       <c r="C107" s="13"/>
       <c r="D107" s="22"/>
       <c r="E107" s="13"/>
@@ -4980,7 +5062,7 @@
       <c r="A108" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B108" s="51"/>
+      <c r="B108" s="55"/>
       <c r="C108" s="13"/>
       <c r="D108" s="22"/>
       <c r="E108" s="13"/>
@@ -5000,7 +5082,7 @@
       <c r="A109" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B109" s="52">
+      <c r="B109" s="50">
         <v>16</v>
       </c>
       <c r="C109" s="16"/>
@@ -5022,7 +5104,7 @@
       <c r="A110" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B110" s="53"/>
+      <c r="B110" s="51"/>
       <c r="C110" s="16"/>
       <c r="D110" s="22"/>
       <c r="E110" s="16"/>
@@ -5042,7 +5124,7 @@
       <c r="A111" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="53"/>
+      <c r="B111" s="51"/>
       <c r="C111" s="16"/>
       <c r="D111" s="22"/>
       <c r="E111" s="16"/>
@@ -5062,7 +5144,7 @@
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B112" s="53"/>
+      <c r="B112" s="51"/>
       <c r="C112" s="16"/>
       <c r="D112" s="22"/>
       <c r="E112" s="16"/>
@@ -5082,7 +5164,7 @@
       <c r="A113" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="53"/>
+      <c r="B113" s="51"/>
       <c r="C113" s="16"/>
       <c r="D113" s="22"/>
       <c r="E113" s="16"/>
@@ -5102,7 +5184,7 @@
       <c r="A114" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B114" s="53"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="16"/>
       <c r="D114" s="22"/>
       <c r="E114" s="16"/>
@@ -5122,7 +5204,7 @@
       <c r="A115" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B115" s="54"/>
+      <c r="B115" s="52"/>
       <c r="C115" s="16"/>
       <c r="D115" s="22"/>
       <c r="E115" s="16"/>
@@ -5140,6 +5222,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="B53:B59"/>
     <mergeCell ref="B95:B101"/>
     <mergeCell ref="B102:B108"/>
     <mergeCell ref="B109:B115"/>
@@ -5148,17 +5241,6 @@
     <mergeCell ref="B74:B80"/>
     <mergeCell ref="B81:B87"/>
     <mergeCell ref="B88:B94"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B53:B59"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5170,9 +5252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202426B2-605C-407B-BD81-2EB34D429EB9}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5253,7 +5333,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="36" t="s">
@@ -5264,7 +5344,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -5275,7 +5355,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="48" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="36" t="s">
@@ -5286,7 +5366,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="36" t="s">
@@ -5297,7 +5377,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="36" t="s">
@@ -5308,7 +5388,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="48" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="36" t="s">
@@ -5319,7 +5399,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="48" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="36" t="s">
@@ -5330,7 +5410,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="36" t="s">
@@ -5341,7 +5421,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="48" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="36" t="s">
@@ -5382,7 +5462,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5395,44 +5475,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5441,11 +5521,11 @@
       <c r="N3" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="55">
+      <c r="O3" s="57">
         <f ca="1">NOW()</f>
-        <v>44733.646704976854</v>
-      </c>
-      <c r="P3" s="56"/>
+        <v>44734.662150925928</v>
+      </c>
+      <c r="P3" s="58"/>
     </row>
     <row r="5" spans="1:16" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -5501,7 +5581,7 @@
       <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="59">
         <v>1</v>
       </c>
       <c r="C6" s="18">
@@ -5551,7 +5631,7 @@
       <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="18">
         <v>1</v>
       </c>
@@ -5599,7 +5679,7 @@
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="58"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="15">
         <v>2</v>
       </c>
@@ -5647,7 +5727,7 @@
       <c r="A9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="58"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="18">
         <v>1</v>
       </c>
@@ -5695,7 +5775,7 @@
       <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="18">
         <v>1</v>
       </c>
@@ -5743,7 +5823,7 @@
       <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="58"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="18">
         <v>10</v>
       </c>
@@ -5791,7 +5871,7 @@
       <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
@@ -5813,7 +5893,7 @@
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="50">
         <v>2</v>
       </c>
       <c r="C13" s="6">
@@ -5863,7 +5943,7 @@
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="53"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="6">
         <v>5</v>
       </c>
@@ -5911,7 +5991,7 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="53"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="15">
         <v>2</v>
       </c>
@@ -5959,7 +6039,7 @@
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="6"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -5979,7 +6059,7 @@
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="6">
         <v>1</v>
       </c>
@@ -6027,7 +6107,7 @@
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="53"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="6">
         <v>1</v>
       </c>
@@ -6075,7 +6155,7 @@
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="54"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -6095,7 +6175,7 @@
       <c r="A20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="57">
+      <c r="B20" s="59">
         <v>3</v>
       </c>
       <c r="C20" s="18">
@@ -6145,7 +6225,7 @@
       <c r="A21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="58"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="18">
         <v>5</v>
       </c>
@@ -6193,7 +6273,7 @@
       <c r="A22" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="58"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="15" t="s">
         <v>94</v>
       </c>
@@ -6241,7 +6321,7 @@
       <c r="A23" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="58"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="18">
         <v>1</v>
       </c>
@@ -6289,7 +6369,7 @@
       <c r="A24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="58"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
@@ -6309,7 +6389,7 @@
       <c r="A25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="58"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="18">
         <v>1</v>
       </c>
@@ -6357,7 +6437,7 @@
       <c r="A26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="59"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
@@ -6377,7 +6457,7 @@
       <c r="A27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="52">
+      <c r="B27" s="50">
         <v>4</v>
       </c>
       <c r="C27" s="35">
@@ -6427,7 +6507,7 @@
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="53"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="5">
         <v>5</v>
       </c>
@@ -6475,7 +6555,7 @@
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="53"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="14" t="s">
         <v>94</v>
       </c>
@@ -6523,7 +6603,7 @@
       <c r="A30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="53"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -6543,7 +6623,7 @@
       <c r="A31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -6567,7 +6647,7 @@
       <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -6591,7 +6671,7 @@
       <c r="A33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="54"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="5">
         <v>1</v>
       </c>
@@ -6633,35 +6713,41 @@
       <c r="A34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="57">
+      <c r="B34" s="59">
         <v>5</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="49">
         <v>1</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="F34" s="62"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="H34" s="62">
+        <v>1</v>
+      </c>
       <c r="I34" s="19"/>
-      <c r="J34" s="61">
-        <v>1</v>
-      </c>
-      <c r="K34" s="61">
+      <c r="J34" s="49">
+        <v>1</v>
+      </c>
+      <c r="K34" s="49">
         <v>1</v>
       </c>
       <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
+      <c r="M34" s="62">
+        <v>1</v>
+      </c>
       <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
+      <c r="O34" s="49">
+        <v>1</v>
+      </c>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="58"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="18">
         <v>6</v>
       </c>
@@ -6669,7 +6755,9 @@
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="H35" s="19">
+        <v>5</v>
+      </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19">
         <v>5</v>
@@ -6678,16 +6766,20 @@
         <v>5</v>
       </c>
       <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
+      <c r="M35" s="19">
+        <v>5</v>
+      </c>
       <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="O35" s="19">
+        <v>5</v>
+      </c>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="58"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="18">
         <v>1</v>
       </c>
@@ -6695,7 +6787,9 @@
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
+      <c r="H36" s="19">
+        <v>2</v>
+      </c>
       <c r="I36" s="19"/>
       <c r="J36" s="14" t="s">
         <v>94</v>
@@ -6704,16 +6798,20 @@
         <v>94</v>
       </c>
       <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
+      <c r="M36" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="O36" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="58"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="18"/>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
@@ -6724,7 +6822,9 @@
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
+      <c r="M37" s="19">
+        <v>1</v>
+      </c>
       <c r="N37" s="19"/>
       <c r="O37" s="19"/>
       <c r="P37" s="19"/>
@@ -6733,7 +6833,7 @@
       <c r="A38" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="58"/>
+      <c r="B38" s="60"/>
       <c r="C38" s="18">
         <v>1</v>
       </c>
@@ -6741,7 +6841,9 @@
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
+      <c r="H38" s="19">
+        <v>1</v>
+      </c>
       <c r="I38" s="19"/>
       <c r="J38" s="19">
         <v>1</v>
@@ -6752,14 +6854,16 @@
       <c r="L38" s="19"/>
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
+      <c r="O38" s="19">
+        <v>1</v>
+      </c>
       <c r="P38" s="19"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="58"/>
+      <c r="B39" s="60"/>
       <c r="C39" s="18">
         <v>1</v>
       </c>
@@ -6767,7 +6871,9 @@
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="H39" s="19">
+        <v>1</v>
+      </c>
       <c r="I39" s="19"/>
       <c r="J39" s="19">
         <v>1</v>
@@ -6776,16 +6882,20 @@
         <v>1</v>
       </c>
       <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
+      <c r="M39" s="19">
+        <v>1</v>
+      </c>
       <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
+      <c r="O39" s="19">
+        <v>1</v>
+      </c>
       <c r="P39" s="19"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="59"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="18"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
@@ -6805,7 +6915,7 @@
       <c r="A41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="52">
+      <c r="B41" s="50">
         <v>6</v>
       </c>
       <c r="C41" s="9"/>
@@ -6827,7 +6937,7 @@
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="53"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -6847,7 +6957,7 @@
       <c r="A43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="53"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -6867,7 +6977,7 @@
       <c r="A44" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="53"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -6887,7 +6997,7 @@
       <c r="A45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="53"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -6907,7 +7017,7 @@
       <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="53"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -6927,7 +7037,7 @@
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="54"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="6"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -6947,7 +7057,7 @@
       <c r="A48" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="57">
+      <c r="B48" s="59">
         <v>7</v>
       </c>
       <c r="C48" s="18"/>
@@ -6969,7 +7079,7 @@
       <c r="A49" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="58"/>
+      <c r="B49" s="60"/>
       <c r="C49" s="18"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
@@ -6989,7 +7099,7 @@
       <c r="A50" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="58"/>
+      <c r="B50" s="60"/>
       <c r="C50" s="18"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19"/>
@@ -7009,7 +7119,7 @@
       <c r="A51" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="58"/>
+      <c r="B51" s="60"/>
       <c r="C51" s="18"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
@@ -7029,7 +7139,7 @@
       <c r="A52" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="58"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="18"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
@@ -7049,7 +7159,7 @@
       <c r="A53" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="58"/>
+      <c r="B53" s="60"/>
       <c r="C53" s="18"/>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
@@ -7069,7 +7179,7 @@
       <c r="A54" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="59"/>
+      <c r="B54" s="61"/>
       <c r="C54" s="18"/>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
@@ -7089,7 +7199,7 @@
       <c r="A55" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="52">
+      <c r="B55" s="50">
         <v>8</v>
       </c>
       <c r="C55" s="5"/>
@@ -7111,7 +7221,7 @@
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="53"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -7131,7 +7241,7 @@
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="53"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -7151,7 +7261,7 @@
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="53"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -7171,7 +7281,7 @@
       <c r="A59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="53"/>
+      <c r="B59" s="51"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -7191,7 +7301,7 @@
       <c r="A60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="53"/>
+      <c r="B60" s="51"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -7211,7 +7321,7 @@
       <c r="A61" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="54"/>
+      <c r="B61" s="52"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -7231,7 +7341,7 @@
       <c r="A62" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="57">
+      <c r="B62" s="59">
         <v>9</v>
       </c>
       <c r="C62" s="18"/>
@@ -7253,7 +7363,7 @@
       <c r="A63" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="58"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="18"/>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
@@ -7273,7 +7383,7 @@
       <c r="A64" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="58"/>
+      <c r="B64" s="60"/>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
@@ -7293,7 +7403,7 @@
       <c r="A65" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="58"/>
+      <c r="B65" s="60"/>
       <c r="C65" s="18"/>
       <c r="D65" s="19"/>
       <c r="E65" s="19"/>
@@ -7313,7 +7423,7 @@
       <c r="A66" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="58"/>
+      <c r="B66" s="60"/>
       <c r="C66" s="18"/>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
@@ -7333,7 +7443,7 @@
       <c r="A67" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B67" s="58"/>
+      <c r="B67" s="60"/>
       <c r="C67" s="18"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
@@ -7353,7 +7463,7 @@
       <c r="A68" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="59"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="18"/>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
@@ -7373,7 +7483,7 @@
       <c r="A69" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="52">
+      <c r="B69" s="50">
         <v>10</v>
       </c>
       <c r="C69" s="5"/>
@@ -7395,7 +7505,7 @@
       <c r="A70" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="53"/>
+      <c r="B70" s="51"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -7415,7 +7525,7 @@
       <c r="A71" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="53"/>
+      <c r="B71" s="51"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -7435,7 +7545,7 @@
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B72" s="53"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -7455,7 +7565,7 @@
       <c r="A73" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B73" s="53"/>
+      <c r="B73" s="51"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -7475,7 +7585,7 @@
       <c r="A74" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B74" s="53"/>
+      <c r="B74" s="51"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
@@ -7495,7 +7605,7 @@
       <c r="A75" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="54"/>
+      <c r="B75" s="52"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
@@ -7515,7 +7625,7 @@
       <c r="A76" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="57">
+      <c r="B76" s="59">
         <v>11</v>
       </c>
       <c r="C76" s="18"/>
@@ -7537,7 +7647,7 @@
       <c r="A77" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="58"/>
+      <c r="B77" s="60"/>
       <c r="C77" s="18"/>
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
@@ -7557,7 +7667,7 @@
       <c r="A78" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="58"/>
+      <c r="B78" s="60"/>
       <c r="C78" s="18"/>
       <c r="D78" s="19"/>
       <c r="E78" s="19"/>
@@ -7577,7 +7687,7 @@
       <c r="A79" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="58"/>
+      <c r="B79" s="60"/>
       <c r="C79" s="18"/>
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
@@ -7597,7 +7707,7 @@
       <c r="A80" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B80" s="58"/>
+      <c r="B80" s="60"/>
       <c r="C80" s="18"/>
       <c r="D80" s="19"/>
       <c r="E80" s="19"/>
@@ -7617,7 +7727,7 @@
       <c r="A81" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B81" s="58"/>
+      <c r="B81" s="60"/>
       <c r="C81" s="18"/>
       <c r="D81" s="19"/>
       <c r="E81" s="19"/>
@@ -7637,7 +7747,7 @@
       <c r="A82" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B82" s="59"/>
+      <c r="B82" s="61"/>
       <c r="C82" s="18"/>
       <c r="D82" s="19"/>
       <c r="E82" s="19"/>
@@ -7657,7 +7767,7 @@
       <c r="A83" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="52">
+      <c r="B83" s="50">
         <v>12</v>
       </c>
       <c r="C83" s="5"/>
@@ -7679,7 +7789,7 @@
       <c r="A84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="53"/>
+      <c r="B84" s="51"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -7699,7 +7809,7 @@
       <c r="A85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="53"/>
+      <c r="B85" s="51"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -7719,7 +7829,7 @@
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B86" s="53"/>
+      <c r="B86" s="51"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -7739,7 +7849,7 @@
       <c r="A87" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="53"/>
+      <c r="B87" s="51"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -7759,7 +7869,7 @@
       <c r="A88" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B88" s="53"/>
+      <c r="B88" s="51"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -7779,7 +7889,7 @@
       <c r="A89" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="54"/>
+      <c r="B89" s="52"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -7799,7 +7909,7 @@
       <c r="A90" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B90" s="57">
+      <c r="B90" s="59">
         <v>13</v>
       </c>
       <c r="C90" s="18"/>
@@ -7821,7 +7931,7 @@
       <c r="A91" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="58"/>
+      <c r="B91" s="60"/>
       <c r="C91" s="18"/>
       <c r="D91" s="19"/>
       <c r="E91" s="19"/>
@@ -7841,7 +7951,7 @@
       <c r="A92" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="58"/>
+      <c r="B92" s="60"/>
       <c r="C92" s="18"/>
       <c r="D92" s="19"/>
       <c r="E92" s="19"/>
@@ -7861,7 +7971,7 @@
       <c r="A93" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B93" s="58"/>
+      <c r="B93" s="60"/>
       <c r="C93" s="18"/>
       <c r="D93" s="19"/>
       <c r="E93" s="19"/>
@@ -7881,7 +7991,7 @@
       <c r="A94" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B94" s="58"/>
+      <c r="B94" s="60"/>
       <c r="C94" s="18"/>
       <c r="D94" s="19"/>
       <c r="E94" s="19"/>
@@ -7901,7 +8011,7 @@
       <c r="A95" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B95" s="58"/>
+      <c r="B95" s="60"/>
       <c r="C95" s="18"/>
       <c r="D95" s="19"/>
       <c r="E95" s="19"/>
@@ -7921,7 +8031,7 @@
       <c r="A96" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B96" s="59"/>
+      <c r="B96" s="61"/>
       <c r="C96" s="18"/>
       <c r="D96" s="19"/>
       <c r="E96" s="19"/>
@@ -7941,7 +8051,7 @@
       <c r="A97" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="52">
+      <c r="B97" s="50">
         <v>14</v>
       </c>
       <c r="C97" s="16"/>
@@ -7963,7 +8073,7 @@
       <c r="A98" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="53"/>
+      <c r="B98" s="51"/>
       <c r="C98" s="16"/>
       <c r="D98" s="16"/>
       <c r="E98" s="16"/>
@@ -7983,7 +8093,7 @@
       <c r="A99" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="53"/>
+      <c r="B99" s="51"/>
       <c r="C99" s="16"/>
       <c r="D99" s="16"/>
       <c r="E99" s="16"/>
@@ -8003,7 +8113,7 @@
       <c r="A100" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="53"/>
+      <c r="B100" s="51"/>
       <c r="C100" s="16"/>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
@@ -8023,7 +8133,7 @@
       <c r="A101" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B101" s="53"/>
+      <c r="B101" s="51"/>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
       <c r="E101" s="16"/>
@@ -8043,7 +8153,7 @@
       <c r="A102" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B102" s="53"/>
+      <c r="B102" s="51"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
       <c r="E102" s="16"/>
@@ -8063,7 +8173,7 @@
       <c r="A103" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="54"/>
+      <c r="B103" s="52"/>
       <c r="C103" s="16"/>
       <c r="D103" s="16"/>
       <c r="E103" s="16"/>
@@ -8083,7 +8193,7 @@
       <c r="A104" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B104" s="57">
+      <c r="B104" s="59">
         <v>15</v>
       </c>
       <c r="C104" s="18"/>
@@ -8105,7 +8215,7 @@
       <c r="A105" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B105" s="58"/>
+      <c r="B105" s="60"/>
       <c r="C105" s="18"/>
       <c r="D105" s="19"/>
       <c r="E105" s="19"/>
@@ -8125,7 +8235,7 @@
       <c r="A106" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="58"/>
+      <c r="B106" s="60"/>
       <c r="C106" s="18"/>
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
@@ -8145,7 +8255,7 @@
       <c r="A107" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="58"/>
+      <c r="B107" s="60"/>
       <c r="C107" s="18"/>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
@@ -8165,7 +8275,7 @@
       <c r="A108" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B108" s="58"/>
+      <c r="B108" s="60"/>
       <c r="C108" s="18"/>
       <c r="D108" s="19"/>
       <c r="E108" s="19"/>
@@ -8185,7 +8295,7 @@
       <c r="A109" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B109" s="58"/>
+      <c r="B109" s="60"/>
       <c r="C109" s="18"/>
       <c r="D109" s="19"/>
       <c r="E109" s="19"/>
@@ -8205,7 +8315,7 @@
       <c r="A110" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="59"/>
+      <c r="B110" s="61"/>
       <c r="C110" s="18"/>
       <c r="D110" s="19"/>
       <c r="E110" s="19"/>
@@ -8225,7 +8335,7 @@
       <c r="A111" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B111" s="52">
+      <c r="B111" s="50">
         <v>16</v>
       </c>
       <c r="C111" s="16"/>
@@ -8247,7 +8357,7 @@
       <c r="A112" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B112" s="53"/>
+      <c r="B112" s="51"/>
       <c r="C112" s="16"/>
       <c r="D112" s="16"/>
       <c r="E112" s="16"/>
@@ -8267,7 +8377,7 @@
       <c r="A113" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="53"/>
+      <c r="B113" s="51"/>
       <c r="C113" s="16"/>
       <c r="D113" s="16"/>
       <c r="E113" s="16"/>
@@ -8287,7 +8397,7 @@
       <c r="A114" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B114" s="53"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="16"/>
       <c r="D114" s="16"/>
       <c r="E114" s="16"/>
@@ -8307,7 +8417,7 @@
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B115" s="53"/>
+      <c r="B115" s="51"/>
       <c r="C115" s="16"/>
       <c r="D115" s="16"/>
       <c r="E115" s="16"/>
@@ -8327,7 +8437,7 @@
       <c r="A116" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B116" s="53"/>
+      <c r="B116" s="51"/>
       <c r="C116" s="16"/>
       <c r="D116" s="16"/>
       <c r="E116" s="16"/>
@@ -8347,7 +8457,7 @@
       <c r="A117" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B117" s="54"/>
+      <c r="B117" s="52"/>
       <c r="C117" s="16"/>
       <c r="D117" s="16"/>
       <c r="E117" s="16"/>
@@ -8365,6 +8475,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="B55:B61"/>
     <mergeCell ref="B97:B103"/>
     <mergeCell ref="B104:B110"/>
     <mergeCell ref="B111:B117"/>
@@ -8373,17 +8494,6 @@
     <mergeCell ref="B76:B82"/>
     <mergeCell ref="B83:B89"/>
     <mergeCell ref="B90:B96"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8395,9 +8505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F8AFC-7FF2-4095-98CA-D6B7FDE000E5}">
   <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8488,7 +8598,7 @@
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="53">
         <v>1</v>
       </c>
       <c r="C6" s="33">
@@ -8526,7 +8636,7 @@
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="12">
         <v>7</v>
       </c>
@@ -8562,7 +8672,7 @@
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="12">
         <v>1</v>
       </c>
@@ -8598,7 +8708,7 @@
       <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="12">
         <v>1</v>
       </c>
@@ -8634,7 +8744,7 @@
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="12">
         <v>1</v>
       </c>
@@ -8670,7 +8780,7 @@
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="12">
         <v>2</v>
       </c>
@@ -8706,7 +8816,7 @@
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="50"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="12">
         <v>1</v>
       </c>
@@ -8742,7 +8852,7 @@
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="50"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -8778,7 +8888,7 @@
       <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="12">
         <v>1</v>
       </c>
@@ -8814,7 +8924,7 @@
       <c r="A15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="52">
+      <c r="B15" s="50">
         <v>2</v>
       </c>
       <c r="C15" s="34">
@@ -8852,7 +8962,7 @@
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="6">
         <v>2</v>
       </c>
@@ -8888,7 +8998,7 @@
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="6">
         <v>1</v>
       </c>
@@ -8924,7 +9034,7 @@
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="53"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="6">
         <v>1</v>
       </c>
@@ -8960,7 +9070,7 @@
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="53"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -8976,7 +9086,7 @@
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="53"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="6">
         <v>1</v>
       </c>
@@ -9012,7 +9122,7 @@
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="54"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="6"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -9028,7 +9138,7 @@
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="53">
         <v>3</v>
       </c>
       <c r="C22" s="33">
@@ -9066,7 +9176,7 @@
       <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="50"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="12">
         <v>1</v>
       </c>
@@ -9102,7 +9212,7 @@
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="12">
         <v>1</v>
       </c>
@@ -9138,7 +9248,7 @@
       <c r="A25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -9154,7 +9264,7 @@
       <c r="A26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -9170,7 +9280,7 @@
       <c r="A27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="50"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -9186,7 +9296,7 @@
       <c r="A28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="12">
         <v>1</v>
       </c>
@@ -9212,7 +9322,7 @@
       <c r="A29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="52">
+      <c r="B29" s="50">
         <v>4</v>
       </c>
       <c r="C29" s="34">
@@ -9250,7 +9360,7 @@
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="53"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="6">
         <v>2</v>
       </c>
@@ -9286,7 +9396,7 @@
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="6">
         <v>1</v>
       </c>
@@ -9322,7 +9432,7 @@
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -9338,7 +9448,7 @@
       <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="53"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="6">
         <v>1</v>
       </c>
@@ -9374,7 +9484,7 @@
       <c r="A34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="53"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="6">
         <v>1</v>
       </c>
@@ -9410,7 +9520,7 @@
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="54"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="6"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -9426,14 +9536,16 @@
       <c r="A36" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="49">
+      <c r="B36" s="53">
         <v>5</v>
       </c>
       <c r="C36" s="33">
         <v>1</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="E36" s="33">
+        <v>1</v>
+      </c>
       <c r="F36" s="13"/>
       <c r="G36" s="33">
         <v>1</v>
@@ -9448,18 +9560,22 @@
       <c r="K36" s="33">
         <v>1</v>
       </c>
-      <c r="L36" s="13"/>
+      <c r="L36" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="50"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="12">
         <v>2</v>
       </c>
       <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
+      <c r="E37" s="12">
+        <v>2</v>
+      </c>
       <c r="F37" s="13"/>
       <c r="G37" s="12">
         <v>2</v>
@@ -9474,18 +9590,22 @@
       <c r="K37" s="12">
         <v>2</v>
       </c>
-      <c r="L37" s="13"/>
+      <c r="L37" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="50"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="12">
         <v>1</v>
       </c>
       <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="12">
+        <v>1</v>
+      </c>
       <c r="F38" s="13"/>
       <c r="G38" s="12">
         <v>1</v>
@@ -9500,18 +9620,22 @@
       <c r="K38" s="12">
         <v>1</v>
       </c>
-      <c r="L38" s="13"/>
+      <c r="L38" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="50"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="12">
         <v>1</v>
       </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="E39" s="12">
+        <v>1</v>
+      </c>
       <c r="F39" s="13"/>
       <c r="G39" s="12">
         <v>1</v>
@@ -9526,34 +9650,38 @@
       <c r="K39" s="12">
         <v>1</v>
       </c>
-      <c r="L39" s="13"/>
+      <c r="L39" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="50"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="13"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="13"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="13"/>
+      <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="50"/>
+      <c r="B41" s="54"/>
       <c r="C41" s="12">
         <v>1</v>
       </c>
       <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="E41" s="12">
+        <v>1</v>
+      </c>
       <c r="F41" s="13"/>
       <c r="G41" s="12">
         <v>1</v>
@@ -9568,13 +9696,15 @@
       <c r="K41" s="12">
         <v>1</v>
       </c>
-      <c r="L41" s="13"/>
+      <c r="L41" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="51"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="12"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -9590,7 +9720,7 @@
       <c r="A43" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="52">
+      <c r="B43" s="50">
         <v>6</v>
       </c>
       <c r="C43" s="9"/>
@@ -9608,7 +9738,7 @@
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="53"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="5"/>
@@ -9624,7 +9754,7 @@
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="53"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="5"/>
@@ -9640,7 +9770,7 @@
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="53"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="9"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -9656,7 +9786,7 @@
       <c r="A47" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="53"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="9"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -9672,7 +9802,7 @@
       <c r="A48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="53"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="9"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -9688,7 +9818,7 @@
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="54"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="9"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -9704,7 +9834,7 @@
       <c r="A50" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="49">
+      <c r="B50" s="53">
         <v>7</v>
       </c>
       <c r="C50" s="11"/>
@@ -9722,7 +9852,7 @@
       <c r="A51" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="50"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
@@ -9738,7 +9868,7 @@
       <c r="A52" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="50"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
@@ -9754,7 +9884,7 @@
       <c r="A53" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="50"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
@@ -9770,7 +9900,7 @@
       <c r="A54" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="50"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
@@ -9786,7 +9916,7 @@
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="50"/>
+      <c r="B55" s="54"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
@@ -9802,7 +9932,7 @@
       <c r="A56" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="51"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
@@ -9818,7 +9948,7 @@
       <c r="A57" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="52">
+      <c r="B57" s="50">
         <v>8</v>
       </c>
       <c r="C57" s="5"/>
@@ -9836,7 +9966,7 @@
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="53"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -9852,7 +9982,7 @@
       <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="53"/>
+      <c r="B59" s="51"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -9868,7 +9998,7 @@
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="53"/>
+      <c r="B60" s="51"/>
       <c r="C60" s="6"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -9884,7 +10014,7 @@
       <c r="A61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="53"/>
+      <c r="B61" s="51"/>
       <c r="C61" s="6"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -9900,7 +10030,7 @@
       <c r="A62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="53"/>
+      <c r="B62" s="51"/>
       <c r="C62" s="6"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -9916,7 +10046,7 @@
       <c r="A63" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="54"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -9932,7 +10062,7 @@
       <c r="A64" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="49">
+      <c r="B64" s="53">
         <v>9</v>
       </c>
       <c r="C64" s="13"/>
@@ -9950,7 +10080,7 @@
       <c r="A65" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="50"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
@@ -9966,7 +10096,7 @@
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="50"/>
+      <c r="B66" s="54"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
@@ -9982,7 +10112,7 @@
       <c r="A67" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="50"/>
+      <c r="B67" s="54"/>
       <c r="C67" s="13"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
@@ -9998,7 +10128,7 @@
       <c r="A68" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="50"/>
+      <c r="B68" s="54"/>
       <c r="C68" s="13"/>
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
@@ -10014,7 +10144,7 @@
       <c r="A69" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="50"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="13"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
@@ -10030,7 +10160,7 @@
       <c r="A70" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="51"/>
+      <c r="B70" s="55"/>
       <c r="C70" s="13"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
@@ -10046,7 +10176,7 @@
       <c r="A71" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="52">
+      <c r="B71" s="50">
         <v>10</v>
       </c>
       <c r="C71" s="5"/>
@@ -10064,7 +10194,7 @@
       <c r="A72" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B72" s="53"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -10080,7 +10210,7 @@
       <c r="A73" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="53"/>
+      <c r="B73" s="51"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -10096,7 +10226,7 @@
       <c r="A74" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="53"/>
+      <c r="B74" s="51"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
@@ -10112,7 +10242,7 @@
       <c r="A75" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B75" s="53"/>
+      <c r="B75" s="51"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
@@ -10128,7 +10258,7 @@
       <c r="A76" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B76" s="53"/>
+      <c r="B76" s="51"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
@@ -10144,7 +10274,7 @@
       <c r="A77" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="54"/>
+      <c r="B77" s="52"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -10160,7 +10290,7 @@
       <c r="A78" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="49">
+      <c r="B78" s="53">
         <v>11</v>
       </c>
       <c r="C78" s="13"/>
@@ -10178,7 +10308,7 @@
       <c r="A79" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="50"/>
+      <c r="B79" s="54"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
@@ -10194,7 +10324,7 @@
       <c r="A80" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B80" s="50"/>
+      <c r="B80" s="54"/>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
@@ -10210,7 +10340,7 @@
       <c r="A81" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="50"/>
+      <c r="B81" s="54"/>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
@@ -10226,7 +10356,7 @@
       <c r="A82" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B82" s="50"/>
+      <c r="B82" s="54"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
       <c r="E82" s="10"/>
@@ -10242,7 +10372,7 @@
       <c r="A83" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B83" s="50"/>
+      <c r="B83" s="54"/>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
@@ -10258,7 +10388,7 @@
       <c r="A84" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="51"/>
+      <c r="B84" s="55"/>
       <c r="C84" s="13"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -10274,7 +10404,7 @@
       <c r="A85" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="52">
+      <c r="B85" s="50">
         <v>12</v>
       </c>
       <c r="C85" s="5"/>
@@ -10292,7 +10422,7 @@
       <c r="A86" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="53"/>
+      <c r="B86" s="51"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -10308,7 +10438,7 @@
       <c r="A87" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="53"/>
+      <c r="B87" s="51"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -10324,7 +10454,7 @@
       <c r="A88" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="53"/>
+      <c r="B88" s="51"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -10340,7 +10470,7 @@
       <c r="A89" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B89" s="53"/>
+      <c r="B89" s="51"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -10356,7 +10486,7 @@
       <c r="A90" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B90" s="53"/>
+      <c r="B90" s="51"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -10372,7 +10502,7 @@
       <c r="A91" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B91" s="54"/>
+      <c r="B91" s="52"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -10388,7 +10518,7 @@
       <c r="A92" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="49">
+      <c r="B92" s="53">
         <v>13</v>
       </c>
       <c r="C92" s="13"/>
@@ -10406,7 +10536,7 @@
       <c r="A93" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="50"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
@@ -10422,7 +10552,7 @@
       <c r="A94" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="50"/>
+      <c r="B94" s="54"/>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
@@ -10438,7 +10568,7 @@
       <c r="A95" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B95" s="50"/>
+      <c r="B95" s="54"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
@@ -10454,7 +10584,7 @@
       <c r="A96" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B96" s="50"/>
+      <c r="B96" s="54"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
@@ -10470,7 +10600,7 @@
       <c r="A97" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B97" s="50"/>
+      <c r="B97" s="54"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
@@ -10486,7 +10616,7 @@
       <c r="A98" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="51"/>
+      <c r="B98" s="55"/>
       <c r="C98" s="13"/>
       <c r="D98" s="10"/>
       <c r="E98" s="10"/>
@@ -10502,7 +10632,7 @@
       <c r="A99" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="52">
+      <c r="B99" s="50">
         <v>14</v>
       </c>
       <c r="C99" s="16"/>
@@ -10520,7 +10650,7 @@
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B100" s="53"/>
+      <c r="B100" s="51"/>
       <c r="C100" s="16"/>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
@@ -10536,7 +10666,7 @@
       <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="53"/>
+      <c r="B101" s="51"/>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
       <c r="E101" s="16"/>
@@ -10552,7 +10682,7 @@
       <c r="A102" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="53"/>
+      <c r="B102" s="51"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
       <c r="E102" s="16"/>
@@ -10568,7 +10698,7 @@
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B103" s="53"/>
+      <c r="B103" s="51"/>
       <c r="C103" s="16"/>
       <c r="D103" s="16"/>
       <c r="E103" s="16"/>
@@ -10584,7 +10714,7 @@
       <c r="A104" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B104" s="53"/>
+      <c r="B104" s="51"/>
       <c r="C104" s="16"/>
       <c r="D104" s="16"/>
       <c r="E104" s="16"/>
@@ -10600,7 +10730,7 @@
       <c r="A105" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="54"/>
+      <c r="B105" s="52"/>
       <c r="C105" s="16"/>
       <c r="D105" s="16"/>
       <c r="E105" s="16"/>
@@ -10616,7 +10746,7 @@
       <c r="A106" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="49">
+      <c r="B106" s="53">
         <v>15</v>
       </c>
       <c r="C106" s="13"/>
@@ -10634,7 +10764,7 @@
       <c r="A107" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B107" s="50"/>
+      <c r="B107" s="54"/>
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
@@ -10650,7 +10780,7 @@
       <c r="A108" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="50"/>
+      <c r="B108" s="54"/>
       <c r="C108" s="13"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
@@ -10666,7 +10796,7 @@
       <c r="A109" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="50"/>
+      <c r="B109" s="54"/>
       <c r="C109" s="13"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
@@ -10682,7 +10812,7 @@
       <c r="A110" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="50"/>
+      <c r="B110" s="54"/>
       <c r="C110" s="13"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
@@ -10698,7 +10828,7 @@
       <c r="A111" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="50"/>
+      <c r="B111" s="54"/>
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
@@ -10714,7 +10844,7 @@
       <c r="A112" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="51"/>
+      <c r="B112" s="55"/>
       <c r="C112" s="13"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
@@ -10730,7 +10860,7 @@
       <c r="A113" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B113" s="52">
+      <c r="B113" s="50">
         <v>16</v>
       </c>
       <c r="C113" s="16"/>
@@ -10748,7 +10878,7 @@
       <c r="A114" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B114" s="53"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="16"/>
       <c r="D114" s="16"/>
       <c r="E114" s="16"/>
@@ -10764,7 +10894,7 @@
       <c r="A115" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B115" s="53"/>
+      <c r="B115" s="51"/>
       <c r="C115" s="16"/>
       <c r="D115" s="16"/>
       <c r="E115" s="16"/>
@@ -10780,7 +10910,7 @@
       <c r="A116" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B116" s="53"/>
+      <c r="B116" s="51"/>
       <c r="C116" s="16"/>
       <c r="D116" s="16"/>
       <c r="E116" s="16"/>
@@ -10796,7 +10926,7 @@
       <c r="A117" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="53"/>
+      <c r="B117" s="51"/>
       <c r="C117" s="16"/>
       <c r="D117" s="16"/>
       <c r="E117" s="16"/>
@@ -10812,7 +10942,7 @@
       <c r="A118" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="53"/>
+      <c r="B118" s="51"/>
       <c r="C118" s="16"/>
       <c r="D118" s="16"/>
       <c r="E118" s="16"/>
@@ -10828,7 +10958,7 @@
       <c r="A119" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B119" s="54"/>
+      <c r="B119" s="52"/>
       <c r="C119" s="16"/>
       <c r="D119" s="16"/>
       <c r="E119" s="16"/>

</xml_diff>

<commit_message>
Miércoles 13/06/2022 controlDiario.xlsx informeMensualJulio2022.xlsx
</commit_message>
<xml_diff>
--- a/controlDiario.xlsx
+++ b/controlDiario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\AHK COORD INGLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87030825-8484-4DEF-92E6-1757DB957FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39BCD9F-1349-4B75-88F1-ED1FB50629A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
   </bookViews>
   <sheets>
     <sheet name="ROSMAIRA (links)" sheetId="1" r:id="rId1"/>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="132">
   <si>
     <t>CURSO</t>
   </si>
@@ -1924,6 +1924,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1964,7 +1965,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -2104,7 +2105,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C16" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}"/>
+  <autoFilter ref="A2:C16" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="01_Lunes"/>
+        <filter val="02_Martes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{A1EA6162-9F94-41F9-B581-C06B3AEA2E9D}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{773B485D-E09A-4C89-9A13-77122C44E990}"/>
@@ -2130,8 +2138,8 @@
   <dimension ref="A1:P115"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3:P3"/>
+      <pane ySplit="5" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2200,7 @@
       </c>
       <c r="O3" s="59">
         <f ca="1">NOW()</f>
-        <v>44753.544625694441</v>
+        <v>44755.876619907409</v>
       </c>
       <c r="P3" s="60"/>
     </row>
@@ -5274,10 +5282,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202426B2-605C-407B-BD81-2EB34D429EB9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5314,7 +5323,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
@@ -5325,7 +5334,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>46</v>
       </c>
@@ -5336,7 +5345,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>47</v>
       </c>
@@ -5347,7 +5356,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>48</v>
       </c>
@@ -5369,7 +5378,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>50</v>
       </c>
@@ -5402,7 +5411,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>53</v>
       </c>
@@ -5424,7 +5433,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
         <v>55</v>
       </c>
@@ -5446,7 +5455,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>57</v>
       </c>
@@ -5458,7 +5467,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C16" xr:uid="{202426B2-605C-407B-BD81-2EB34D429EB9}"/>
+  <autoFilter ref="A2:C16" xr:uid="{202426B2-605C-407B-BD81-2EB34D429EB9}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="01_Lunes"/>
+        <filter val="01_Lunes &amp; Miércoles"/>
+        <filter val="02_Martes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{DD95A364-B1CC-4080-9273-D870CFBF8027}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{AFF5CC48-0E1B-447C-A9B8-DC1E941AE79B}"/>
@@ -5488,7 +5505,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O48" sqref="O48"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5549,7 +5566,7 @@
       </c>
       <c r="O3" s="59">
         <f ca="1">NOW()</f>
-        <v>44753.544625694441</v>
+        <v>44755.876619907409</v>
       </c>
       <c r="P3" s="60"/>
     </row>
@@ -8820,11 +8837,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F8AFC-7FF2-4095-98CA-D6B7FDE000E5}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8836,7 +8853,7 @@
     <col min="5" max="12" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
@@ -8852,7 +8869,7 @@
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>43</v>
       </c>
@@ -8868,12 +8885,20 @@
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="K3" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="59">
+        <f ca="1">NOW()</f>
+        <v>44755.876619907409</v>
+      </c>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="5" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -8911,7 +8936,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
@@ -8949,7 +8974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -8985,7 +9010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -9021,7 +9046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
@@ -9057,7 +9082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -9093,7 +9118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -9129,7 +9154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -9165,7 +9190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -9201,7 +9226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
@@ -9237,7 +9262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>6</v>
       </c>
@@ -9275,7 +9300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -10273,7 +10298,9 @@
       <c r="E50" s="50">
         <v>1</v>
       </c>
-      <c r="F50" s="12"/>
+      <c r="F50" s="50">
+        <v>1</v>
+      </c>
       <c r="G50" s="50">
         <v>1</v>
       </c>
@@ -10307,7 +10334,9 @@
       <c r="E51" s="12">
         <v>1</v>
       </c>
-      <c r="F51" s="12"/>
+      <c r="F51" s="12">
+        <v>1</v>
+      </c>
       <c r="G51" s="12">
         <v>1</v>
       </c>
@@ -10341,7 +10370,9 @@
       <c r="E52" s="12">
         <v>1</v>
       </c>
-      <c r="F52" s="12"/>
+      <c r="F52" s="12">
+        <v>1</v>
+      </c>
       <c r="G52" s="12">
         <v>1</v>
       </c>
@@ -10432,48 +10463,102 @@
       <c r="B57" s="56">
         <v>8</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
+      <c r="C57" s="33">
+        <v>1</v>
+      </c>
+      <c r="D57" s="33">
+        <v>1</v>
+      </c>
+      <c r="E57" s="33">
+        <v>1</v>
+      </c>
+      <c r="F57" s="33">
+        <v>1</v>
+      </c>
+      <c r="G57" s="33">
+        <v>1</v>
+      </c>
+      <c r="H57" s="33">
+        <v>1</v>
+      </c>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33">
+        <v>1</v>
+      </c>
+      <c r="K57" s="33">
+        <v>1</v>
+      </c>
+      <c r="L57" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="57"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
+      <c r="C58" s="5">
+        <v>2</v>
+      </c>
+      <c r="D58" s="5">
+        <v>2</v>
+      </c>
+      <c r="E58" s="5">
+        <v>2</v>
+      </c>
+      <c r="F58" s="5">
+        <v>2</v>
+      </c>
+      <c r="G58" s="5">
+        <v>2</v>
+      </c>
+      <c r="H58" s="5">
+        <v>2</v>
+      </c>
       <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
+      <c r="J58" s="5">
+        <v>2</v>
+      </c>
+      <c r="K58" s="5">
+        <v>2</v>
+      </c>
+      <c r="L58" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="57"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
+      <c r="C59" s="6">
+        <v>1</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1</v>
+      </c>
+      <c r="E59" s="6">
+        <v>1</v>
+      </c>
+      <c r="F59" s="6">
+        <v>1</v>
+      </c>
+      <c r="G59" s="6">
+        <v>1</v>
+      </c>
+      <c r="H59" s="6">
+        <v>1</v>
+      </c>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6">
+        <v>1</v>
+      </c>
+      <c r="K59" s="6">
+        <v>1</v>
+      </c>
+      <c r="L59" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -11452,11 +11537,7 @@
       <c r="L119" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B6:B14"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B29:B35"/>
+  <mergeCells count="17">
     <mergeCell ref="B113:B119"/>
     <mergeCell ref="B36:B42"/>
     <mergeCell ref="B43:B49"/>
@@ -11469,6 +11550,11 @@
     <mergeCell ref="B92:B98"/>
     <mergeCell ref="B99:B105"/>
     <mergeCell ref="B106:B112"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Martes 19 de julio 2022
</commit_message>
<xml_diff>
--- a/controlDiario.xlsx
+++ b/controlDiario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\AHK COORD INGLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39BCD9F-1349-4B75-88F1-ED1FB50629A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D742A1E1-692F-43F1-A174-2F65C8D47918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
   </bookViews>
   <sheets>
     <sheet name="ROSMAIRA (links)" sheetId="1" r:id="rId1"/>
@@ -1927,7 +1927,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1972,7 +1972,7 @@
       <c r="B4" s="18"/>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -2109,7 +2109,6 @@
     <filterColumn colId="2">
       <filters>
         <filter val="01_Lunes"/>
-        <filter val="02_Martes"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2200,7 +2199,7 @@
       </c>
       <c r="O3" s="59">
         <f ca="1">NOW()</f>
-        <v>44755.876619907409</v>
+        <v>44761.890328125002</v>
       </c>
       <c r="P3" s="60"/>
     </row>
@@ -5286,7 +5285,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5367,7 +5366,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>49</v>
       </c>
@@ -5422,7 +5421,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>54</v>
       </c>
@@ -5444,7 +5443,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>56</v>
       </c>
@@ -5472,7 +5471,6 @@
       <filters>
         <filter val="01_Lunes"/>
         <filter val="01_Lunes &amp; Miércoles"/>
-        <filter val="02_Martes"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5566,7 +5564,7 @@
       </c>
       <c r="O3" s="59">
         <f ca="1">NOW()</f>
-        <v>44755.876619907409</v>
+        <v>44761.890328125002</v>
       </c>
       <c r="P3" s="60"/>
     </row>
@@ -8839,9 +8837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F8AFC-7FF2-4095-98CA-D6B7FDE000E5}">
   <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8894,7 +8892,7 @@
       </c>
       <c r="L3" s="59">
         <f ca="1">NOW()</f>
-        <v>44755.876619907409</v>
+        <v>44761.890328125002</v>
       </c>
       <c r="M3" s="60"/>
     </row>
@@ -10481,7 +10479,9 @@
       <c r="H57" s="33">
         <v>1</v>
       </c>
-      <c r="I57" s="33"/>
+      <c r="I57" s="33">
+        <v>1</v>
+      </c>
       <c r="J57" s="33">
         <v>1</v>
       </c>
@@ -10515,7 +10515,9 @@
       <c r="H58" s="5">
         <v>2</v>
       </c>
-      <c r="I58" s="5"/>
+      <c r="I58" s="5">
+        <v>2</v>
+      </c>
       <c r="J58" s="5">
         <v>2</v>
       </c>
@@ -10549,7 +10551,9 @@
       <c r="H59" s="6">
         <v>1</v>
       </c>
-      <c r="I59" s="6"/>
+      <c r="I59" s="6">
+        <v>1</v>
+      </c>
       <c r="J59" s="6">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Files that had not been committed
</commit_message>
<xml_diff>
--- a/controlDiario.xlsx
+++ b/controlDiario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\COORD_INGLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8430E9F8-5B3B-4BD6-83B8-A57B51EAD10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A88AB9-56C5-4E20-A6A0-F9C20D87B1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0F7888BE-47E6-4C2F-86A4-AF0D51AADF96}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="CLASS LINKS (4)" sheetId="24" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CLASS LINKS'!$A$2:$E$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CLASS LINKS'!$A$2:$E$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'CLASS LINKS (2)'!$B$2:$D$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CLASS LINKS (3)'!$B$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CLASS LINKS (4)'!$B$2:$D$2</definedName>
@@ -34,8 +34,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="82">
   <si>
     <t>CURSO</t>
   </si>
@@ -244,6 +248,51 @@
   </si>
   <si>
     <t>VI</t>
+  </si>
+  <si>
+    <t>CASTRO MAGAYANES ISRAEL EDUARDO</t>
+  </si>
+  <si>
+    <t>4A ADMEMP-R</t>
+  </si>
+  <si>
+    <t>4A ECON-R</t>
+  </si>
+  <si>
+    <t>4A FIN</t>
+  </si>
+  <si>
+    <t>4A ADMPUBL</t>
+  </si>
+  <si>
+    <t>4A ZOOT-R</t>
+  </si>
+  <si>
+    <t>4B ADMPUBL</t>
+  </si>
+  <si>
+    <t>4B ECON-R</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPWS</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPWR</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPVW</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPWQ</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPWP</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPVX</t>
+  </si>
+  <si>
+    <t>https://sga.uteq.edu.ec/adm_seguimientoacademico?action=seguimientoaulavirtual&amp;id=OPPQQRRSSTTUUVVPVPVY</t>
   </si>
 </sst>
 </file>
@@ -331,7 +380,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,13 +396,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,11 +727,11 @@
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="112.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -717,7 +759,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -726,16 +768,16 @@
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -749,16 +791,16 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="D5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -772,16 +814,16 @@
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="D6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -795,16 +837,16 @@
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="D7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -818,16 +860,16 @@
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -841,16 +883,16 @@
       <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="D9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -864,16 +906,16 @@
       <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="D10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -887,16 +929,16 @@
       <c r="C11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="D11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -910,16 +952,16 @@
       <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -933,16 +975,16 @@
       <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -956,16 +998,16 @@
       <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -979,16 +1021,16 @@
       <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="D15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1002,16 +1044,16 @@
       <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1025,16 +1067,16 @@
       <c r="C17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="D17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1048,16 +1090,16 @@
       <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1071,16 +1113,16 @@
       <c r="C19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="D19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1094,16 +1136,16 @@
       <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1117,16 +1159,16 @@
       <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="D21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1140,16 +1182,16 @@
       <c r="C22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="D22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1163,16 +1205,16 @@
       <c r="C23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="D23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1186,16 +1228,16 @@
       <c r="C24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="10" t="s">
+      <c r="D24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1206,16 +1248,16 @@
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="D25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1226,16 +1268,16 @@
       <c r="B26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="D26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1246,16 +1288,16 @@
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="10" t="s">
+      <c r="D27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1266,16 +1308,16 @@
       <c r="B28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="10" t="s">
+      <c r="D28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1286,16 +1328,16 @@
       <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="10" t="s">
+      <c r="D29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1306,16 +1348,16 @@
       <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="10" t="s">
+      <c r="D30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1350,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1404,7 @@
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="112.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="9"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1383,7 +1425,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1509,7 +1551,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>63</v>
@@ -1739,8 +1781,127 @@
         <v>64</v>
       </c>
     </row>
+    <row r="24" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:E23" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}"/>
+  <autoFilter ref="A2:E30" xr:uid="{AD822270-F21C-4E8C-A827-2D8279C5D454}"/>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" xr:uid="{50E5235C-36F0-4963-9869-432C28248FEE}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{4412421F-924C-4913-965B-A85CAF10DB8E}"/>
@@ -1763,9 +1924,16 @@
     <hyperlink ref="C19" r:id="rId19" xr:uid="{16DBD981-2430-434E-B55B-02DE8D716A60}"/>
     <hyperlink ref="C20" r:id="rId20" xr:uid="{06E0CAE2-7922-4265-AACA-14D54EE1B166}"/>
     <hyperlink ref="C22" r:id="rId21" xr:uid="{B0AD2142-03A7-44D9-946E-2022DDCD3491}"/>
+    <hyperlink ref="C24" r:id="rId22" xr:uid="{07CB1E10-FFB2-45F3-8861-99CD15ED3F12}"/>
+    <hyperlink ref="C27" r:id="rId23" xr:uid="{8B8CB565-7B48-44EC-A3BE-9D3F455C14A5}"/>
+    <hyperlink ref="C28" r:id="rId24" xr:uid="{E0D04B9A-8EE0-4BE1-88E5-E57F9144ED3E}"/>
+    <hyperlink ref="C29" r:id="rId25" xr:uid="{F98F0681-A5C9-48ED-B534-13086BE9637C}"/>
+    <hyperlink ref="C25" r:id="rId26" xr:uid="{0A50F81D-5FD3-4B9B-A08F-8CAD4EEB59F6}"/>
+    <hyperlink ref="C26" r:id="rId27" xr:uid="{2FAF2A3B-0884-4444-8376-725592B0705C}"/>
+    <hyperlink ref="C30" r:id="rId28" xr:uid="{FC303AD4-6ECF-4449-8AFA-0F9ED8BE3C65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 
@@ -1782,7 +1950,7 @@
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="112.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1800,7 +1968,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1914,7 +2082,7 @@
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="112.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2046,7 +2214,7 @@
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="112.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>